<commit_message>
PJ edits to document
</commit_message>
<xml_diff>
--- a/Submissions/Case1/iea37-cs1-aepranks.xlsx
+++ b/Submissions/Case1/iea37-cs1-aepranks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
   <si>
     <t>AEP</t>
   </si>
@@ -153,12 +153,33 @@
   </si>
   <si>
     <t>Wish I would've limited wall time</t>
+  </si>
+  <si>
+    <t>1hr</t>
+  </si>
+  <si>
+    <t>4hrs</t>
+  </si>
+  <si>
+    <t>2min total, 2s per opt</t>
+  </si>
+  <si>
+    <t>161s</t>
+  </si>
+  <si>
+    <t>8hrs</t>
+  </si>
+  <si>
+    <t>8 hrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -202,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -210,12 +231,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="178" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,16 +548,16 @@
       <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -551,7 +574,7 @@
       <c r="E3">
         <v>11</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -574,6 +597,9 @@
       <c r="G4">
         <v>50</v>
       </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
       <c r="I4" s="2" t="s">
         <v>36</v>
       </c>
@@ -629,6 +655,9 @@
       <c r="G6">
         <v>150</v>
       </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>35</v>
       </c>
@@ -831,6 +860,18 @@
       <c r="E15" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="F15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -845,7 +886,7 @@
       <c r="E16" s="4">
         <v>11</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -868,6 +909,9 @@
       <c r="G17">
         <v>50</v>
       </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
       <c r="I17" s="2" t="s">
         <v>36</v>
       </c>
@@ -886,13 +930,13 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>6000</v>
+        <v>424</v>
       </c>
       <c r="G18">
         <v>300</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>35</v>
@@ -948,6 +992,21 @@
       <c r="C21">
         <v>5</v>
       </c>
+      <c r="D21" s="1">
+        <v>820394.24028599996</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>30072</v>
+      </c>
+      <c r="G21">
+        <v>1000</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
       <c r="I21" s="2" t="s">
         <v>36</v>
       </c>
@@ -963,7 +1022,7 @@
         <v>776000.14246</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>35</v>
@@ -980,7 +1039,7 @@
         <v>777475.78272599995</v>
       </c>
       <c r="E23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>35</v>
@@ -1020,7 +1079,7 @@
         <v>813544.21048000001</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>35</v>
@@ -1068,6 +1127,18 @@
       <c r="E28" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="F28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
@@ -1082,7 +1153,7 @@
       <c r="E29" s="4">
         <v>11</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1105,6 +1176,9 @@
       <c r="G30">
         <v>50</v>
       </c>
+      <c r="H30" t="s">
+        <v>43</v>
+      </c>
       <c r="I30" s="2" t="s">
         <v>36</v>
       </c>
@@ -1185,6 +1259,21 @@
       <c r="C34">
         <v>5</v>
       </c>
+      <c r="D34" s="8">
+        <v>1336164.5497999999</v>
+      </c>
+      <c r="E34">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>30113</v>
+      </c>
+      <c r="G34">
+        <v>500</v>
+      </c>
+      <c r="H34" t="s">
+        <v>47</v>
+      </c>
       <c r="I34" s="2" t="s">
         <v>36</v>
       </c>
@@ -1202,6 +1291,9 @@
       <c r="E35">
         <v>8</v>
       </c>
+      <c r="H35" t="s">
+        <v>26</v>
+      </c>
       <c r="I35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1217,7 +1309,7 @@
         <v>1332883.4328399999</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>35</v>
@@ -1231,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="1">
-        <v>1425678.1431177701</v>
+        <v>1445967.377229</v>
       </c>
       <c r="E37">
         <v>6</v>

</xml_diff>